<commit_message>
finished copy of ux
</commit_message>
<xml_diff>
--- a/Assignment/Real/Data Matrix.xlsx
+++ b/Assignment/Real/Data Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukeh\Desktop\User Experience\User_Experience_Term_1\Assignment\Real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2DCAAC-85C2-4D1A-B368-A60DE9CCA016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7579C707-A606-4F81-8DDA-5B2FC4B9620F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,9 +241,6 @@
     <t>7. A definition of sustainability</t>
   </si>
   <si>
-    <t>8. Whether participants mentioned finance</t>
-  </si>
-  <si>
     <t>9. Mention of university in terms of struggling in eating or sustainable food</t>
   </si>
   <si>
@@ -275,6 +272,9 @@
   </si>
   <si>
     <t>"I don’t get as much help from the government for being a student, a lot I rely on working on myself to feed myself, so essentially the more hours I put in the more choice I have, but its quite difficult to balance everything…  I would say I'd go with the cheapest option, even if its not healthy as much but um, just cheapest"</t>
+  </si>
+  <si>
+    <t>8. The mention of finance from participants</t>
   </si>
 </sst>
 </file>
@@ -448,6 +448,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -455,29 +467,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -704,8 +704,8 @@
   </sheetPr>
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="106" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="91" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -735,46 +735,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="19" t="s">
         <v>68</v>
       </c>
       <c r="P1" s="5"/>
@@ -787,20 +787,20 @@
       <c r="W1" s="24"/>
     </row>
     <row r="2" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -811,35 +811,35 @@
       <c r="W2" s="25"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="13" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="P3" s="7"/>
@@ -851,21 +851,21 @@
       <c r="V3" s="7"/>
     </row>
     <row r="4" spans="1:23" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="11"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="17"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -875,35 +875,35 @@
       <c r="V4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="19" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="10" t="s">
+      <c r="J5" s="12"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="16" t="s">
         <v>30</v>
       </c>
       <c r="P5" s="7"/>
@@ -915,21 +915,21 @@
       <c r="V5" s="7"/>
     </row>
     <row r="6" spans="1:23" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -939,43 +939,43 @@
       <c r="V6" s="4"/>
     </row>
     <row r="7" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13" t="s">
+      <c r="K7" s="18"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="21" t="s">
         <v>12</v>
       </c>
       <c r="P7" s="7"/>
@@ -987,21 +987,21 @@
       <c r="V7" s="7"/>
     </row>
     <row r="8" spans="1:23" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="14"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1011,43 +1011,43 @@
       <c r="V8" s="4"/>
     </row>
     <row r="9" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="19" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J9" s="10" t="s">
+      <c r="I9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="19" t="s">
+      <c r="K9" s="12"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="P9" s="7"/>
@@ -1059,21 +1059,21 @@
       <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:23" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="14"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="15"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1083,35 +1083,35 @@
       <c r="V10" s="4"/>
     </row>
     <row r="11" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="19" t="s">
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="19" t="s">
+      <c r="K11" s="12"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="16" t="s">
         <v>47</v>
       </c>
       <c r="P11" s="7"/>
@@ -1123,21 +1123,21 @@
       <c r="V11" s="7"/>
     </row>
     <row r="12" spans="1:23" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="11"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="17"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -1147,37 +1147,37 @@
       <c r="V12" s="4"/>
     </row>
     <row r="13" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="19" t="s">
+      <c r="I13" s="22"/>
+      <c r="J13" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="10" t="s">
+      <c r="K13" s="12"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="O13" s="10" t="s">
+      <c r="O13" s="16" t="s">
         <v>53</v>
       </c>
       <c r="P13" s="7"/>
@@ -1189,21 +1189,21 @@
       <c r="V13" s="7"/>
     </row>
     <row r="14" spans="1:23" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -1235,19 +1235,19 @@
     <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1259,37 +1259,37 @@
     <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1310,11 +1310,92 @@
     </row>
     <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="105">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
@@ -1339,87 +1420,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O7:O8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1428,21 +1428,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <link xmlns="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </link>
-    <TaxCatchAll xmlns="da5699a2-2791-44c0-bb0a-d0c081c141e6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001BC1D44B3665304E9EFFB6B26E5C1EDB" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ebe7ffaa3beae6c2692551344dbac989">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5" xmlns:ns3="da5699a2-2791-44c0-bb0a-d0c081c141e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbc6f3879e7a0016066cbb62231de351" ns2:_="" ns3:_="">
     <xsd:import namespace="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5"/>
@@ -1698,6 +1683,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <link xmlns="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </link>
+    <TaxCatchAll xmlns="da5699a2-2791-44c0-bb0a-d0c081c141e6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1708,23 +1708,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D011DE68-88AB-4AB5-8382-5E6B89E1EF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="da5699a2-2791-44c0-bb0a-d0c081c141e6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D90BBA-494B-4484-9073-5C34692BB072}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1743,6 +1726,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D011DE68-88AB-4AB5-8382-5E6B89E1EF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="da5699a2-2791-44c0-bb0a-d0c081c141e6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3ca5950f-9dc6-4fa2-8e6b-e8b0d1a55fc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEA30742-A1E2-4ABD-9C52-733279A899BB}">
   <ds:schemaRefs>

</xml_diff>